<commit_message>
+Question_1 completed Pending work : Annotation and prject analyses
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rencita.Monteiro\Documents\UiPath\Rencita_Day_11\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED59E49E-D6DD-4E50-B413-B29F87198F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36FEA08-64F0-4A3F-8D5E-8C74D75453AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -554,7 +554,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>